<commit_message>
Cleaned up all the spreadsheets. Still some owrk to do on the turn effect.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Properties/CurvesConfiguration.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Properties/CurvesConfiguration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2017\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Properties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Properties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C71BC2B-419A-473A-9BCF-02AE2C6622B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AF9647-177B-4A20-AFF3-F0B5D3FDFC80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="270" windowWidth="14955" windowHeight="12525" tabRatio="724" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="0" windowWidth="26370" windowHeight="14820" tabRatio="724" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FxCurves" sheetId="12" r:id="rId1"/>
@@ -79,7 +79,15 @@
     <definedName name="Spreads" localSheetId="2">NZDCurves!#REF!</definedName>
     <definedName name="Spreads" localSheetId="4">USDCurves!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -23039,7 +23047,7 @@
   <protectedRanges>
     <protectedRange sqref="M11 R11 W11 C14 AB11 H12" name="Range2_1_1_1_2"/>
   </protectedRanges>
-  <sortState ref="AI19:AI91">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AI19:AI91">
     <sortCondition ref="AI19:AI91"/>
   </sortState>
   <mergeCells count="4">
@@ -28042,7 +28050,7 @@
   <protectedRanges>
     <protectedRange sqref="F13 C13 I13 L13" name="Range2_1_1_1_2"/>
   </protectedRanges>
-  <sortState ref="K15:K99">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K15:K99">
     <sortCondition ref="K15:K99"/>
   </sortState>
   <dataValidations count="8">

</xml_diff>